<commit_message>
added authors to single book view - and tested
</commit_message>
<xml_diff>
--- a/stories.xlsx
+++ b/stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="stories" sheetId="1" state="visible" r:id="rId2"/>
@@ -402,26 +402,26 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="15:15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="89.4897959183674"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="91.9387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="69.4948979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.9183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.7551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.7959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="95.6122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="98.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="98.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="74.1836734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9744897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.9744897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="40.3061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9744897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="53.1581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.9744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="17.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,26 +777,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated readme, added pagination tests, added search result tests
</commit_message>
<xml_diff>
--- a/stories.xlsx
+++ b/stories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="stories" sheetId="1" state="visible" r:id="rId2"/>
@@ -402,26 +402,26 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="21:21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="95.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="98.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="98.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9744897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="74.1836734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="54.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.9744897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="40.3061224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9744897959184"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="53.1581632653061"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="17.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="108.877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="112.040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="84.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9438775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="45.9132653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.9183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="60.6122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.9183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.97959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,49 +840,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -920,48 +920,48 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="E21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>